<commit_message>
Added initial NMEA handlers for ROT and TRA2
</commit_message>
<xml_diff>
--- a/UM982 Config/UM982 Data Output.xlsx
+++ b/UM982 Config/UM982 Data Output.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chris/Code/Basic_Dual_WiFi_UM982/UM982 Config/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{376B0C34-487B-7E4E-8D3B-AB57B1496BDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07E7B8AB-BC54-CC42-952C-16C3027C32AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31320" yWindow="7600" windowWidth="35480" windowHeight="18780" xr2:uid="{7DBC0B9E-FAB4-0E4A-8594-97EF7A87F9DA}"/>
+    <workbookView xWindow="31320" yWindow="4760" windowWidth="35480" windowHeight="21620" xr2:uid="{7DBC0B9E-FAB4-0E4A-8594-97EF7A87F9DA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
 <connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
   <connection id="1" xr16:uid="{1151DAB1-B726-E045-AB96-18CF857F9FE3}" name="panda_sample1" type="6" refreshedVersion="8" background="1" saveData="1">
-    <textPr codePage="10000" sourceFile="/Users/chris/Downloads/panda_sample.txt" tab="0" comma="1" delimiter="*">
+    <textPr sourceFile="/Users/chris/Downloads/panda_sample.txt" tab="0" comma="1" delimiter="*">
       <textFields count="17">
         <textField/>
         <textField/>
@@ -68,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="39">
   <si>
     <t>$PANDA</t>
   </si>
@@ -182,6 +182,9 @@
   </si>
   <si>
     <t>$GPTRA2</t>
+  </si>
+  <si>
+    <t>$GPVTG</t>
   </si>
 </sst>
 </file>
@@ -569,10 +572,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{171CC2A3-EE6D-2B40-83AA-43E9154863D0}">
-  <dimension ref="A1:S23"/>
+  <dimension ref="A1:S24"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="P23" sqref="P23"/>
+      <selection activeCell="P27" sqref="P27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -1563,70 +1566,81 @@
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="E21" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="G21" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="H21" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="J21" s="4" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="L21" s="4" t="s">
         <v>34</v>
       </c>
       <c r="M21" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="N21" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="O21" s="4" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="P22" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="G22" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="H22" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="J22" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="L22" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="M22" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="N22" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="O22" s="4" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="P23" s="4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A24" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="B23" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="G23" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="H23" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="K23" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="M23" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="N23" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="O23" s="4" t="s">
+      <c r="B24" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="G24" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="H24" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="K24" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="M24" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="N24" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="O24" s="4" t="s">
         <v>34</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added all ready to buildpanda.
</commit_message>
<xml_diff>
--- a/UM982 Config/UM982 Data Output.xlsx
+++ b/UM982 Config/UM982 Data Output.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chris/Code/Basic_Dual_WiFi_UM982/UM982 Config/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chris/Code/Basic_WiFi_UM982/UM982 Config/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{07E7B8AB-BC54-CC42-952C-16C3027C32AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EA6B944C-3EAF-E64E-A5C7-E4E5E52FDE9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="31320" yWindow="4760" windowWidth="35480" windowHeight="21620" xr2:uid="{7DBC0B9E-FAB4-0E4A-8594-97EF7A87F9DA}"/>
   </bookViews>
@@ -68,7 +68,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="38">
   <si>
     <t>$PANDA</t>
   </si>
@@ -179,9 +179,6 @@
   </si>
   <si>
     <t>$GPROT</t>
-  </si>
-  <si>
-    <t>$GPTRA2</t>
   </si>
   <si>
     <t>$GPVTG</t>
@@ -572,10 +569,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{171CC2A3-EE6D-2B40-83AA-43E9154863D0}">
-  <dimension ref="A1:S24"/>
+  <dimension ref="A1:S23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="P27" sqref="P27"/>
+      <selection activeCell="A24" sqref="A24:XFD24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="19" x14ac:dyDescent="0.25"/>
@@ -1566,7 +1563,7 @@
     </row>
     <row r="21" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="L21" s="4" t="s">
         <v>34</v>
@@ -1574,73 +1571,29 @@
       <c r="M21" s="4" t="s">
         <v>34</v>
       </c>
+      <c r="N21" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="O21" s="4" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="22" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="E22" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="G22" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="H22" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="J22" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="L22" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="M22" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="N22" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="O22" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="P22" s="4" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="23" spans="1:17" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="P23" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="L23" s="4" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.25">
-      <c r="A24" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="G24" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="H24" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="K24" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="M24" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="N24" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="O24" s="4" t="s">
+      <c r="M23" s="4" t="s">
         <v>34</v>
       </c>
     </row>

</xml_diff>